<commit_message>
Updating of the total Cost of the BOM
</commit_message>
<xml_diff>
--- a/Hybrid_Dewatering_BOM.xlsx
+++ b/Hybrid_Dewatering_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ari-Tech-Forge\Github\Hybrid-Dewatering-System-PLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A43C89CF-49DD-4F95-83B4-2A01CEE009C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6503819-0257-4D57-9E50-04726423CEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLC_BOM" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <sheet name="Totals_Summary" sheetId="5" r:id="rId5"/>
     <sheet name="Notes" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>Item</t>
   </si>
@@ -268,6 +279,12 @@
   </si>
   <si>
     <t>If you want, I can refine this into an RFQ-ready Excel with columns: PN, Vendor, MOQ, Lead time, Exact price.</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>TOTAL Cost Approx</t>
   </si>
 </sst>
 </file>
@@ -323,10 +340,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,15 +650,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="118" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,7 +692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -684,7 +715,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -707,7 +738,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -730,7 +761,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -753,7 +784,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -776,7 +807,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -799,7 +830,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -822,7 +853,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -845,7 +876,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -868,7 +899,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -891,7 +922,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -913,8 +944,14 @@
       <c r="G12">
         <v>60000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -937,7 +974,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -960,7 +997,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -983,7 +1020,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1050,6 +1087,23 @@
       </c>
       <c r="G18">
         <v>100000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C2:C18)</f>
+        <v>479500</v>
+      </c>
+      <c r="F19">
+        <f>SUM(F2:F18)</f>
+        <v>510500</v>
+      </c>
+      <c r="G19">
+        <f>SUM(G2:G18)</f>
+        <v>1988000</v>
       </c>
     </row>
   </sheetData>
@@ -1061,9 +1115,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1166,9 +1231,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1221,9 +1294,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1303,9 +1387,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1437,9 +1528,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>